<commit_message>
Atualização dos arquivos .xlsx
</commit_message>
<xml_diff>
--- a/data/historico_dividendos.xlsx
+++ b/data/historico_dividendos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C143"/>
+  <dimension ref="A1:C141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -813,7 +813,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -822,13 +822,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.998729</v>
+        <v>0.948793</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -837,13 +837,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.948793</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -852,13 +852,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.948793</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -867,13 +867,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -882,13 +882,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.95</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -897,13 +897,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.07</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -927,43 +927,43 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1.07</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>KNCR11.SA</t>
+          <t>MXRF11.SA</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.04</v>
+        <v>0.099845</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>KNCR11.SA</t>
+          <t>MXRF11.SA</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1.16</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -972,13 +972,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.099845</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -987,13 +987,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1002,13 +1002,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1023,7 +1023,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1032,13 +1032,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1047,13 +1047,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1062,13 +1062,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1077,13 +1077,13 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1098,7 +1098,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1107,43 +1107,43 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>MXRF11.SA</t>
+          <t>PORD11.SA</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MXRF11.SA</t>
+          <t>PORD11.SA</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.1</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1152,13 +1152,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.091</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1167,13 +1167,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.091</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1188,7 +1188,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1197,13 +1197,13 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.089</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1218,7 +1218,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1227,13 +1227,13 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.091</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1242,13 +1242,13 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.089</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1257,13 +1257,13 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.089</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1272,13 +1272,13 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.082</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1287,43 +1287,43 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.09</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>PORD11.SA</t>
+          <t>RZTR11.SA</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.08799999999999999</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>PORD11.SA</t>
+          <t>RZTR11.SA</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.092</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1338,7 +1338,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1353,7 +1353,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1368,7 +1368,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1383,7 +1383,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1392,13 +1392,13 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.9</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1407,13 +1407,13 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.9</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1422,13 +1422,13 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.15</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1437,13 +1437,13 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1458,7 +1458,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1473,37 +1473,37 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>RZTR11.SA</t>
+          <t>VGHF11.SA</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.05</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>RZTR11.SA</t>
+          <t>VGHF11.SA</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.05</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1518,7 +1518,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1533,7 +1533,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1542,13 +1542,13 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1563,7 +1563,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1572,13 +1572,13 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1593,7 +1593,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1608,7 +1608,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1623,7 +1623,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1638,7 +1638,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1653,12 +1653,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>04/06/2024</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>VGHF11.SA</t>
+          <t>GGRC11.SA</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1668,22 +1668,22 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>02/07/2024</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>VGHF11.SA</t>
+          <t>GGRC11.SA</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.09</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>04/06/2024</t>
+          <t>02/08/2024</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1692,13 +1692,13 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>02/07/2024</t>
+          <t>03/09/2024</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1707,13 +1707,13 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.093</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>02/08/2024</t>
+          <t>02/10/2024</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1722,13 +1722,13 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.091</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>03/09/2024</t>
+          <t>04/11/2024</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1737,13 +1737,13 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.091</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>02/10/2024</t>
+          <t>03/12/2024</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1758,7 +1758,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>04/11/2024</t>
+          <t>03/01/2025</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1767,13 +1767,13 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.1</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>03/12/2024</t>
+          <t>04/02/2025</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1782,13 +1782,13 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.1</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>03/01/2025</t>
+          <t>06/03/2025</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1797,13 +1797,13 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.095</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>04/02/2025</t>
+          <t>02/04/2025</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1812,13 +1812,13 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.095</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>06/03/2025</t>
+          <t>05/05/2025</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1833,37 +1833,37 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>02/04/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>GGRC11.SA</t>
+          <t>XPLG11.SA</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.1</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>05/05/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>GGRC11.SA</t>
+          <t>XPLG11.SA</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.1</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1878,7 +1878,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1893,7 +1893,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1923,7 +1923,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1938,7 +1938,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1953,7 +1953,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1962,13 +1962,13 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1977,13 +1977,13 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1998,7 +1998,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2013,37 +2013,37 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>20/05/2024</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>XPLG11.SA</t>
+          <t>XPML11.SA</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.82</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>19/06/2024</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>XPLG11.SA</t>
+          <t>XPML11.SA</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0.82</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>20/05/2024</t>
+          <t>19/07/2024</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2058,7 +2058,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>19/06/2024</t>
+          <t>19/08/2024</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2073,7 +2073,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>19/07/2024</t>
+          <t>19/09/2024</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2088,7 +2088,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>19/08/2024</t>
+          <t>21/10/2024</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2103,7 +2103,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>19/09/2024</t>
+          <t>18/11/2024</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2118,7 +2118,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>21/10/2024</t>
+          <t>17/12/2024</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -2133,7 +2133,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>18/11/2024</t>
+          <t>20/01/2025</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2148,7 +2148,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>17/12/2024</t>
+          <t>19/02/2025</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2163,7 +2163,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>20/01/2025</t>
+          <t>19/03/2025</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2178,7 +2178,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>19/02/2025</t>
+          <t>17/04/2025</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2193,37 +2193,37 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>19/03/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>XPML11.SA</t>
+          <t>GARE11.SA</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.92</v>
+        <v>0.08699999999999999</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>17/04/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>XPML11.SA</t>
+          <t>GARE11.SA</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.92</v>
+        <v>0.08699999999999999</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2238,7 +2238,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2253,7 +2253,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2262,13 +2262,13 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2277,13 +2277,13 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2292,13 +2292,13 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.09</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2313,7 +2313,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2322,13 +2322,13 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.092</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2337,13 +2337,13 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.092</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2358,7 +2358,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -2373,37 +2373,37 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>01/04/2025</t>
+          <t>03/06/2024</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>GARE11.SA</t>
+          <t>VISC11.SA</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.083</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>02/05/2025</t>
+          <t>01/07/2024</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>GARE11.SA</t>
+          <t>VISC11.SA</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0.083</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>03/06/2024</t>
+          <t>01/08/2024</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2412,13 +2412,13 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>01/07/2024</t>
+          <t>02/09/2024</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -2427,13 +2427,13 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.85</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>01/08/2024</t>
+          <t>01/10/2024</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -2442,13 +2442,13 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>02/09/2024</t>
+          <t>01/11/2024</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2457,13 +2457,13 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.83</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>01/10/2024</t>
+          <t>02/12/2024</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2478,7 +2478,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>01/11/2024</t>
+          <t>02/01/2025</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2493,7 +2493,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>02/12/2024</t>
+          <t>03/02/2025</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2508,7 +2508,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>02/01/2025</t>
+          <t>05/03/2025</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2523,7 +2523,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>01/04/2025</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2538,7 +2538,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>05/03/2025</t>
+          <t>02/05/2025</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2547,36 +2547,6 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>01/04/2025</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>VISC11.SA</t>
-        </is>
-      </c>
-      <c r="C142" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>02/05/2025</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>VISC11.SA</t>
-        </is>
-      </c>
-      <c r="C143" t="n">
         <v>0.08</v>
       </c>
     </row>

</xml_diff>